<commit_message>
Added magnetic uncertainty and corresponding tests
</commit_message>
<xml_diff>
--- a/tests/samples/MASSREF4tests.xlsx
+++ b/tests/samples/MASSREF4tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908C147A-17D0-421A-B8A7-03E8CF81CE1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B818DF94-0E0F-4269-BD7A-0A41BD8FF5A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26190" yWindow="2400" windowWidth="14400" windowHeight="7365" tabRatio="843" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="843" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mettler A" sheetId="13" r:id="rId1"/>
@@ -388,6 +388,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>g)</t>
     </r>
@@ -411,6 +412,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -434,6 +436,7 @@
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -514,6 +517,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -636,7 +640,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -815,6 +819,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1228,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2373,7 +2380,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4400,8 +4407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE9B5D4-F934-48BA-9C7B-67137F0D6D60}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5202,7 +5209,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5231,8 +5238,8 @@
         <v>30</v>
       </c>
       <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
-        <v>22</v>
+      <c r="D1" s="56" t="s">
+        <v>24</v>
       </c>
       <c r="E1" s="41" t="s">
         <v>1</v>
@@ -5328,10 +5335,10 @@
         <v>15</v>
       </c>
       <c r="C4" s="48"/>
-      <c r="D4" s="49">
-        <v>10000.003261553</v>
-      </c>
-      <c r="E4" s="50">
+      <c r="D4" s="19">
+        <v>10000.00503</v>
+      </c>
+      <c r="E4" s="20">
         <v>155.87700000000001</v>
       </c>
       <c r="F4" s="24">

</xml_diff>

<commit_message>
added test cases from TP MSLT.M.001.008 appendices C and D
Test cases are for a single circular weighing and a matrix least squares analysis for a set of 9 masses respectively.
To use a relative uncertainty of 0.1 ppm for no buoyancy correction, a change was made in the FinalMassCalc class to include REL_UNC as a class variable so that the value could be changed in this class instance only.
</commit_message>
<xml_diff>
--- a/tests/samples/MASSREF4tests.xlsx
+++ b/tests/samples/MASSREF4tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B818DF94-0E0F-4269-BD7A-0A41BD8FF5A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FEB06C-3023-4068-BF0E-588C887A53DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="843" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34620" yWindow="4180" windowWidth="10520" windowHeight="15020" tabRatio="843" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mettler A" sheetId="13" r:id="rId1"/>
@@ -18,16 +18,22 @@
     <sheet name="CUSTOM" sheetId="15" r:id="rId3"/>
     <sheet name="Mettler A (2)" sheetId="17" r:id="rId4"/>
     <sheet name="Mettler B (2)" sheetId="18" r:id="rId5"/>
+    <sheet name="Mettler 76a" sheetId="20" r:id="rId6"/>
+    <sheet name="W5 SS" sheetId="21" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'Mettler 76a'!$A:$C,'Mettler 76a'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Mettler A'!$A:$C,'Mettler A'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Mettler A (2)'!$A:$C,'Mettler A (2)'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Mettler B'!$A:$C,'Mettler B'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Mettler B (2)'!$A:$C,'Mettler B (2)'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'W5 SS'!$A:$C,'W5 SS'!$1:$3</definedName>
+    <definedName name="WeightSet" localSheetId="5">'Mettler 76a'!$B$4:$H$21</definedName>
     <definedName name="WeightSet" localSheetId="0">'Mettler A'!$B$5:$H$36</definedName>
     <definedName name="WeightSet" localSheetId="3">'Mettler A (2)'!$B$5:$H$36</definedName>
     <definedName name="WeightSet" localSheetId="1">'Mettler B'!$B$8:$H$36</definedName>
     <definedName name="WeightSet" localSheetId="4">'Mettler B (2)'!$B$8:$H$36</definedName>
+    <definedName name="WeightSet" localSheetId="6">'W5 SS'!$B$5:$H$36</definedName>
     <definedName name="WeightSet">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -212,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="41">
   <si>
     <t>ID:</t>
   </si>
@@ -450,6 +456,18 @@
   <si>
     <t>···</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Mettler 76a</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>W5 SS</t>
+  </si>
 </sst>
 </file>
 
@@ -640,7 +658,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -823,6 +841,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5208,7 +5227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1FE45F-5790-4499-A796-54814D075F0F}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -6003,4 +6022,1749 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F65443D-EC23-4028-B732-6F2DA2E7A0B6}">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.7265625" customWidth="1"/>
+    <col min="12" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="60.7265625" customWidth="1"/>
+    <col min="16" max="16" width="0.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="33">
+        <v>35065</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13">
+        <v>100</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4">
+        <v>100.00005910799999</v>
+      </c>
+      <c r="E4">
+        <v>4.008</v>
+      </c>
+      <c r="F4" s="21">
+        <v>34</v>
+      </c>
+      <c r="G4" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H4" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="20">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21">
+        <v>50</v>
+      </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="13">
+        <v>50</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="57">
+        <v>50.000053126000005</v>
+      </c>
+      <c r="E5">
+        <v>2.6240000000000001</v>
+      </c>
+      <c r="F5" s="21">
+        <v>14</v>
+      </c>
+      <c r="G5" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H5" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="20">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>50</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="13">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="57">
+        <v>19.999998345999998</v>
+      </c>
+      <c r="E6">
+        <v>2.0880000000000001</v>
+      </c>
+      <c r="F6" s="21">
+        <v>14</v>
+      </c>
+      <c r="G6" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H6" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="20">
+        <v>0</v>
+      </c>
+      <c r="N6" s="21">
+        <v>50</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="13">
+        <v>10</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="57">
+        <v>10.000010290999999</v>
+      </c>
+      <c r="E7">
+        <v>1.7470000000000001</v>
+      </c>
+      <c r="F7" s="21">
+        <v>14</v>
+      </c>
+      <c r="G7" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="20">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>50</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="13">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="57">
+        <v>4.9999977819999994</v>
+      </c>
+      <c r="E8">
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="F8" s="21">
+        <v>14</v>
+      </c>
+      <c r="G8" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H8" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="20">
+        <v>0</v>
+      </c>
+      <c r="N8" s="21">
+        <v>50</v>
+      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="57">
+        <v>1.9999962910000002</v>
+      </c>
+      <c r="E9">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="F9" s="21">
+        <v>14</v>
+      </c>
+      <c r="G9" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="20">
+        <v>0</v>
+      </c>
+      <c r="N9" s="21">
+        <v>50</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="57">
+        <v>0.99995660099999994</v>
+      </c>
+      <c r="E10">
+        <v>0.752</v>
+      </c>
+      <c r="F10" s="21">
+        <v>14</v>
+      </c>
+      <c r="G10" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H10" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="20">
+        <v>0</v>
+      </c>
+      <c r="N10" s="21">
+        <v>50</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:16" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="0"/>
+  <pageMargins left="0.75" right="0.5" top="0.75" bottom="0.5" header="0.375" footer="0.25"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;A&amp;RPage &amp;P of &amp;N</oddHeader>
+    <oddFooter>&amp;L&amp;F&amp;R&amp;T  &amp;D</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8520A4B3-5717-4848-9B55-AE1CAF888F1F}">
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.7265625" customWidth="1"/>
+    <col min="12" max="14" width="12.7265625" customWidth="1"/>
+    <col min="15" max="15" width="60.7265625" customWidth="1"/>
+    <col min="16" max="16" width="0.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="33">
+        <v>35065</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="19">
+        <v>10000.00364074</v>
+      </c>
+      <c r="E4" s="20">
+        <v>155.87700000000001</v>
+      </c>
+      <c r="F4" s="21">
+        <v>33</v>
+      </c>
+      <c r="G4" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H4" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="20">
+        <v>427.00529078689408</v>
+      </c>
+      <c r="N4" s="21">
+        <v>50</v>
+      </c>
+      <c r="O4" s="31"/>
+    </row>
+    <row r="5" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="19">
+        <v>5000.0028770019999</v>
+      </c>
+      <c r="E5" s="20">
+        <v>78.076999999999998</v>
+      </c>
+      <c r="F5" s="21">
+        <v>33</v>
+      </c>
+      <c r="G5" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H5" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="20">
+        <v>213.77517311418552</v>
+      </c>
+      <c r="N5" s="21">
+        <v>50</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="19">
+        <v>1999.999615211</v>
+      </c>
+      <c r="E6" s="20">
+        <v>31.314</v>
+      </c>
+      <c r="F6" s="21">
+        <v>33</v>
+      </c>
+      <c r="G6" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H6" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="20">
+        <v>85.469199300098751</v>
+      </c>
+      <c r="N6" s="21">
+        <v>50</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="19">
+        <v>1000.000541002</v>
+      </c>
+      <c r="E7" s="20">
+        <v>14.785</v>
+      </c>
+      <c r="F7" s="21">
+        <v>18</v>
+      </c>
+      <c r="G7" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H7" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I7" s="21">
+        <v>102</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="20">
+        <v>42.044148213514802</v>
+      </c>
+      <c r="N7" s="21">
+        <v>50</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13">
+        <v>500</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="19">
+        <v>500.00011696799999</v>
+      </c>
+      <c r="E8" s="20">
+        <v>7.6219999999999999</v>
+      </c>
+      <c r="F8" s="21">
+        <v>34</v>
+      </c>
+      <c r="G8" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H8" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="20">
+        <v>20.95166201044681</v>
+      </c>
+      <c r="N8" s="21">
+        <v>50</v>
+      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13">
+        <v>200</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="19">
+        <v>200.000195848</v>
+      </c>
+      <c r="E9" s="20">
+        <v>3.7669999999999999</v>
+      </c>
+      <c r="F9" s="21">
+        <v>34</v>
+      </c>
+      <c r="G9" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="20">
+        <v>8.1087108716490821</v>
+      </c>
+      <c r="N9" s="21">
+        <v>50</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13">
+        <v>100</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="19">
+        <v>100.000058368</v>
+      </c>
+      <c r="E10" s="20">
+        <v>2.7090000000000001</v>
+      </c>
+      <c r="F10" s="21">
+        <v>34</v>
+      </c>
+      <c r="G10" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H10" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I10" s="21"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="20">
+        <v>3.62698883372971</v>
+      </c>
+      <c r="N10" s="21">
+        <v>50</v>
+      </c>
+      <c r="O10" s="17"/>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="19">
+        <v>50.000035719000003</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1.377</v>
+      </c>
+      <c r="F11" s="21">
+        <v>14</v>
+      </c>
+      <c r="G11" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H11" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I11" s="21"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="20">
+        <v>2.2746762406988821</v>
+      </c>
+      <c r="N11" s="21">
+        <v>50</v>
+      </c>
+      <c r="O11" s="17"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="13">
+        <v>20</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="19">
+        <v>20.000006814999999</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="F12" s="21">
+        <v>14</v>
+      </c>
+      <c r="G12" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H12" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="20">
+        <v>2.0414546284451194</v>
+      </c>
+      <c r="N12" s="21">
+        <v>50</v>
+      </c>
+      <c r="O12" s="17"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="19">
+        <v>10.000013709999999</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0.318</v>
+      </c>
+      <c r="F13" s="21">
+        <v>14</v>
+      </c>
+      <c r="G13" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H13" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="20">
+        <v>1.655739109884163</v>
+      </c>
+      <c r="N13" s="21">
+        <v>50</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="19">
+        <v>5.0000117030000002</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0.246</v>
+      </c>
+      <c r="F14" s="21">
+        <v>14</v>
+      </c>
+      <c r="G14" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H14" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="20">
+        <v>1.3192603988599068</v>
+      </c>
+      <c r="N14" s="21">
+        <v>50</v>
+      </c>
+      <c r="O14" s="17"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="19">
+        <v>2.0000093849999998</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F15" s="21">
+        <v>14</v>
+      </c>
+      <c r="G15" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H15" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="20">
+        <v>0.99318125234017574</v>
+      </c>
+      <c r="N15" s="21">
+        <v>50</v>
+      </c>
+      <c r="O15" s="17"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="19">
+        <v>1.0000066750000001</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.1148</v>
+      </c>
+      <c r="F16" s="21">
+        <v>14</v>
+      </c>
+      <c r="G16" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H16" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="20">
+        <v>0.82908983831669292</v>
+      </c>
+      <c r="N16" s="21">
+        <v>50</v>
+      </c>
+      <c r="O16" s="17"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="19">
+        <v>0.49999992700000001</v>
+      </c>
+      <c r="E17" s="20">
+        <v>9.8100000000000007E-2</v>
+      </c>
+      <c r="F17" s="21">
+        <v>14</v>
+      </c>
+      <c r="G17" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H17" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I17" s="21"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="20">
+        <v>0.66581182777118042</v>
+      </c>
+      <c r="N17" s="21">
+        <v>50</v>
+      </c>
+      <c r="O17" s="17"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="19">
+        <v>0.20000657299999999</v>
+      </c>
+      <c r="E18" s="20">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="F18" s="21">
+        <v>14</v>
+      </c>
+      <c r="G18" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H18" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I18" s="21"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="20">
+        <v>0.49959827861993278</v>
+      </c>
+      <c r="N18" s="21">
+        <v>50</v>
+      </c>
+      <c r="O18" s="17"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="19">
+        <v>9.9997197999999995E-2</v>
+      </c>
+      <c r="E19" s="20">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="F19" s="21">
+        <v>14</v>
+      </c>
+      <c r="G19" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H19" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I19" s="21"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="20">
+        <v>0.41747052590572187</v>
+      </c>
+      <c r="N19" s="21">
+        <v>50</v>
+      </c>
+      <c r="O19" s="17"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="19">
+        <v>5.0003101000000001E-2</v>
+      </c>
+      <c r="E20" s="20">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="F20" s="21">
+        <v>14</v>
+      </c>
+      <c r="G20" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H20" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="20">
+        <v>0.3297413986747797</v>
+      </c>
+      <c r="N20" s="21">
+        <v>50</v>
+      </c>
+      <c r="O20" s="17"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="19">
+        <v>2.0001313E-2</v>
+      </c>
+      <c r="E21" s="20">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="F21" s="21">
+        <v>14</v>
+      </c>
+      <c r="G21" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H21" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="20">
+        <v>0.24788473127645438</v>
+      </c>
+      <c r="N21" s="21">
+        <v>50</v>
+      </c>
+      <c r="O21" s="17"/>
+      <c r="P21" s="10"/>
+    </row>
+    <row r="22" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="19">
+        <v>1.0001782000000001E-2</v>
+      </c>
+      <c r="E22" s="20">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="F22" s="21">
+        <v>14</v>
+      </c>
+      <c r="G22" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H22" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I22" s="21"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="20">
+        <v>0.24916964100788844</v>
+      </c>
+      <c r="N22" s="21">
+        <v>50</v>
+      </c>
+      <c r="O22" s="17"/>
+      <c r="P22" s="10"/>
+    </row>
+    <row r="23" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="19">
+        <v>5.0012650000000004E-3</v>
+      </c>
+      <c r="E23" s="20">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F23" s="21">
+        <v>14</v>
+      </c>
+      <c r="G23" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H23" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="20">
+        <v>0.25063120316512866</v>
+      </c>
+      <c r="N23" s="21">
+        <v>50</v>
+      </c>
+      <c r="O23" s="17"/>
+      <c r="P23" s="10"/>
+    </row>
+    <row r="24" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="19">
+        <v>2.0007419999999998E-3</v>
+      </c>
+      <c r="E24" s="20">
+        <v>2.86E-2</v>
+      </c>
+      <c r="F24" s="21">
+        <v>14</v>
+      </c>
+      <c r="G24" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H24" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I24" s="21"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="20">
+        <v>0.25037180352427868</v>
+      </c>
+      <c r="N24" s="21">
+        <v>50</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="19">
+        <v>1.0016179999999999E-3</v>
+      </c>
+      <c r="E25" s="20">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="F25" s="21">
+        <v>14</v>
+      </c>
+      <c r="G25" s="32">
+        <v>8012</v>
+      </c>
+      <c r="H25" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="I25" s="21"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="20">
+        <v>0.25038320630585431</v>
+      </c>
+      <c r="N25" s="21">
+        <v>50</v>
+      </c>
+      <c r="O25" s="17"/>
+      <c r="P25" s="10"/>
+    </row>
+    <row r="26" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="10"/>
+    </row>
+    <row r="27" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="10"/>
+    </row>
+    <row r="29" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="10"/>
+    </row>
+    <row r="31" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="10"/>
+    </row>
+    <row r="32" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="10"/>
+    </row>
+    <row r="35" spans="1:16" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" gridLinesSet="0"/>
+  <pageMargins left="0.75" right="0.5" top="0.75" bottom="0.5" header="0.375" footer="0.25"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;A&amp;RPage &amp;P of &amp;N</oddHeader>
+    <oddFooter>&amp;L&amp;F&amp;R&amp;T  &amp;D</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>